<commit_message>
Fixed printer crash on code
</commit_message>
<xml_diff>
--- a/ExcelChartTool/bin/Debug/O&M_Copy.xlsx
+++ b/ExcelChartTool/bin/Debug/O&M_Copy.xlsx
@@ -1,12 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:bookViews>
+    <x:workbookView xWindow="0" yWindow="0" windowWidth="20310" windowHeight="9540"/>
+  </x:bookViews>
   <x:sheets>
     <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="RAW Data_all" sheetId="1" r:id="rId1"/>
     <x:sheet name="SumVol" sheetId="2" r:id="rId6"/>
     <x:sheet name="WeeklyFlowRates" sheetId="3" r:id="rId7"/>
-    <x:sheet name="records" sheetId="4" r:id="R90abaee580b548fe"/>
-    <x:sheet name="stationReport" sheetId="5" r:id="Rf46ff3d229a048db"/>
+    <x:sheet name="records" sheetId="4" r:id="R6b20de02f28742ef"/>
+    <x:sheet name="stationReport" sheetId="5" r:id="R5c17a7e5cc1942ae"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -3775,10 +3778,10 @@
   </x:sheetPr>
   <x:dimension ref="A1:I1488"/>
   <x:sheetViews>
-    <x:sheetView workbookViewId="0">
+    <x:sheetView tabSelected="1" workbookViewId="0">
       <x:pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <x:selection activeCell="E597" sqref="E597"/>
-      <x:selection pane="bottomLeft" activeCell="C49" sqref="C49"/>
+      <x:selection pane="bottomLeft" activeCell="J23" sqref="J23"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>